<commit_message>
Save photos to folder and add new lifts to excel
</commit_message>
<xml_diff>
--- a/middleman-bot/middleman-bot/lifts.xlsx
+++ b/middleman-bot/middleman-bot/lifts.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15990" windowWidth="29040" xWindow="-120" yWindow="-120"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="11505" windowWidth="12150" xWindow="13830" yWindow="3630"/>
   </bookViews>
   <sheets>
     <sheet name="lifts" sheetId="1" state="visible" r:id="rId1"/>
@@ -405,16 +405,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="9.140625"/>
-    <col customWidth="1" max="16384" min="2" style="1" width="9.140625"/>
+    <col customWidth="1" max="2" min="1" style="1" width="9.140625"/>
+    <col customWidth="1" max="16384" min="3" style="1" width="9.140625"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="2">
@@ -489,6 +489,131 @@
         </is>
       </c>
       <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D4" s="1" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>047G</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>047G-P</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>Note</t>
         </is>
@@ -514,8 +639,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="1" width="9.140625"/>
-    <col customWidth="1" max="16384" min="2" style="1" width="9.140625"/>
+    <col customWidth="1" max="2" min="1" style="1" width="9.140625"/>
+    <col customWidth="1" max="16384" min="3" style="1" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>

<commit_message>
user_data from multiple elements to single lift element
</commit_message>
<xml_diff>
--- a/middleman-bot/middleman-bot/lifts.xlsx
+++ b/middleman-bot/middleman-bot/lifts.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -841,6 +841,156 @@
       <c r="E17" t="inlineStr">
         <is>
           <t>Konde</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>15</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>16</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>047G</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>047G-P</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Huomenna on RYÖpäivä</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>17</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Best taustakuva</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>18</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>19</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>20</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>NONE</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Note</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Bug: If conversation starts without photo, error ocurs : FIXED
</commit_message>
<xml_diff>
--- a/middleman-bot/middleman-bot/lifts.xlsx
+++ b/middleman-bot/middleman-bot/lifts.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
@@ -1666,6 +1666,31 @@
       <c r="E50" t="inlineStr">
         <is>
           <t>Läähpuuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>48</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>WAREHOUSE</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Teinipeili selfie piti ottaa pitkästä aikaa</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Add lift photo to state update
</commit_message>
<xml_diff>
--- a/middleman-bot/middleman-bot/lifts.xlsx
+++ b/middleman-bot/middleman-bot/lifts.xlsx
@@ -405,7 +405,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5:E5"/>
@@ -525,7 +525,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SITE</t>
+          <t>WAREHOUSE</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -541,6 +541,31 @@
       <c r="E5" t="inlineStr">
         <is>
           <t>🅱ottu ❤️</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>SHORE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>S</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>N</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Send contact after messages
</commit_message>
<xml_diff>
--- a/middleman-bot/middleman-bot/lifts.xlsx
+++ b/middleman-bot/middleman-bot/lifts.xlsx
@@ -417,18 +417,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="1" width="9.140625"/>
     <col customWidth="1" max="2" min="2" style="1" width="16.28515625"/>
-    <col customWidth="1" max="15" min="3" style="1" width="9.140625"/>
-    <col customWidth="1" max="16384" min="16" style="1" width="9.140625"/>
+    <col customWidth="1" max="16" min="3" style="1" width="9.140625"/>
+    <col customWidth="1" max="16384" min="17" style="1" width="9.140625"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="2">
@@ -514,33 +514,10 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Note</t>
-        </is>
-      </c>
-    </row>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
-    <row r="20"/>
-    <row r="21"/>
-    <row r="22"/>
-    <row r="23"/>
-    <row r="24"/>
-    <row r="25"/>
-    <row r="26"/>
+          <t>N</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -561,8 +538,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="15" min="1" style="1" width="9.140625"/>
-    <col customWidth="1" max="16384" min="16" style="1" width="9.140625"/>
+    <col customWidth="1" max="16" min="1" style="1" width="9.140625"/>
+    <col customWidth="1" max="16384" min="17" style="1" width="9.140625"/>
   </cols>
   <sheetData>
     <row customFormat="1" r="1" s="2">

</xml_diff>